<commit_message>
forgot about this one
</commit_message>
<xml_diff>
--- a/extraction/raw extraction/kappen2000/kappen2000.xlsx
+++ b/extraction/raw extraction/kappen2000/kappen2000.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/margaretslein/lichen/extraction/raw extraction/kappen2000/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A20B1409-02BE-1648-933C-6931B465E498}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D7C91C1-ADB9-1046-B2CF-3E0503BA925D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30440" yWindow="-9580" windowWidth="27240" windowHeight="15640" xr2:uid="{AB4CDE7F-4415-8B4B-94F5-33E1E0797D74}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16740" xr2:uid="{AB4CDE7F-4415-8B4B-94F5-33E1E0797D74}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="10">
   <si>
     <t>x</t>
   </si>
@@ -56,15 +56,31 @@
   <si>
     <t>figure 4</t>
   </si>
+  <si>
+    <t>ppfd</t>
+  </si>
+  <si>
+    <t>ppfd_units</t>
+  </si>
+  <si>
+    <t>umol * m^-2 * s^-1</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -90,8 +106,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -406,15 +423,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C4B56C5-7777-D143-AA3C-E59C33F32B1E}">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B15"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="K32" sqref="K32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -427,13 +444,19 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>-8.1442751320669302</v>
+        <v>-8.0323467583396599</v>
       </c>
       <c r="B2">
-        <v>-7.1788338760292404E-3</v>
+        <v>-7.4298057627246701E-3</v>
       </c>
       <c r="C2" t="s">
         <v>6</v>
@@ -441,13 +464,19 @@
       <c r="D2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>-4.0353949219403198</v>
+        <v>-4.1126310445747398</v>
       </c>
       <c r="B3">
-        <v>-0.13743076938211299</v>
+        <v>-0.136466591938182</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
@@ -455,13 +484,19 @@
       <c r="D3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>0.76328293311559703</v>
+        <v>0.81222594350389998</v>
       </c>
       <c r="B4">
-        <v>-0.240420843457645</v>
+        <v>-0.242726408569472</v>
       </c>
       <c r="C4" t="s">
         <v>6</v>
@@ -469,13 +504,19 @@
       <c r="D4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>4.33346777763568</v>
+        <v>4.4071521292507496</v>
       </c>
       <c r="B5">
-        <v>-0.41335474604782901</v>
+        <v>-0.41263990296653902</v>
       </c>
       <c r="C5" t="s">
         <v>6</v>
@@ -483,13 +524,19 @@
       <c r="D5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>9.3442397174702201</v>
+        <v>9.3969888282051102</v>
       </c>
       <c r="B6">
-        <v>-0.68252043717352096</v>
+        <v>-0.68192002235040305</v>
       </c>
       <c r="C6" t="s">
         <v>6</v>
@@ -497,13 +544,19 @@
       <c r="D6" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>14.707190146872099</v>
+        <v>14.6805152858364</v>
       </c>
       <c r="B7">
-        <v>-1.2415324682990101</v>
+        <v>-1.24253561243854</v>
       </c>
       <c r="C7" t="s">
         <v>6</v>
@@ -511,13 +564,19 @@
       <c r="D7" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>-7.30140773021947</v>
+        <v>-7.3476067010326798</v>
       </c>
       <c r="B8">
-        <v>2.3993389275279699E-2</v>
+        <v>2.13470206843446E-2</v>
       </c>
       <c r="C8" t="s">
         <v>6</v>
@@ -525,13 +584,19 @@
       <c r="D8" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E8">
+        <v>170</v>
+      </c>
+      <c r="F8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>-3.2373860092668201</v>
+        <v>-3.1978998797303002</v>
       </c>
       <c r="B9">
-        <v>0.203006797635092</v>
+        <v>0.20625095823949599</v>
       </c>
       <c r="C9" t="s">
         <v>6</v>
@@ -539,13 +604,19 @@
       <c r="D9" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E9" s="1">
+        <v>170</v>
+      </c>
+      <c r="F9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>1.8906475952505</v>
+        <v>1.9498887590415099</v>
       </c>
       <c r="B10">
-        <v>0.33593696201784401</v>
+        <v>0.33852173883416697</v>
       </c>
       <c r="C10" t="s">
         <v>6</v>
@@ -553,13 +624,19 @@
       <c r="D10" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E10" s="1">
+        <v>170</v>
+      </c>
+      <c r="F10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>5.6186241429175698</v>
+        <v>5.6294466571495603</v>
       </c>
       <c r="B11">
-        <v>0.213306542846743</v>
+        <v>0.215513428981251</v>
       </c>
       <c r="C11" t="s">
         <v>6</v>
@@ -567,13 +644,19 @@
       <c r="D11" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E11" s="1">
+        <v>170</v>
+      </c>
+      <c r="F11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>10.715178105909301</v>
+        <v>10.7079217872146</v>
       </c>
       <c r="B12">
-        <v>3.6949229240652103E-2</v>
+        <v>3.5938836211742903E-2</v>
       </c>
       <c r="C12" t="s">
         <v>6</v>
@@ -581,13 +664,19 @@
       <c r="D12" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E12" s="1">
+        <v>170</v>
+      </c>
+      <c r="F12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>15.478047868729799</v>
+        <v>15.4797875348799</v>
       </c>
       <c r="B13">
-        <v>-0.41785535104718902</v>
+        <v>-0.41888098069211199</v>
       </c>
       <c r="C13" t="s">
         <v>6</v>
@@ -595,13 +684,19 @@
       <c r="D13" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E13" s="1">
+        <v>170</v>
+      </c>
+      <c r="F13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>20.465210077420199</v>
+        <v>20.448064271039499</v>
       </c>
       <c r="B14">
-        <v>-0.91898665066451501</v>
+        <v>-0.91846770264422894</v>
       </c>
       <c r="C14" t="s">
         <v>6</v>
@@ -609,19 +704,491 @@
       <c r="D14" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E14" s="1">
+        <v>170</v>
+      </c>
+      <c r="F14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>25.7561508268324</v>
+        <v>25.7355974474203</v>
       </c>
       <c r="B15">
-        <v>-1.43549378768949</v>
+        <v>-1.4362829506621599</v>
       </c>
       <c r="C15" t="s">
         <v>6</v>
       </c>
       <c r="D15" t="s">
         <v>5</v>
+      </c>
+      <c r="E15" s="1">
+        <v>170</v>
+      </c>
+      <c r="F15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>-6.4970375493599803</v>
+      </c>
+      <c r="B16">
+        <v>0.10724820873096599</v>
+      </c>
+      <c r="C16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" t="s">
+        <v>5</v>
+      </c>
+      <c r="E16" s="1">
+        <v>400</v>
+      </c>
+      <c r="F16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>-2.2953796672651801</v>
+      </c>
+      <c r="B17">
+        <v>0.41852937067940399</v>
+      </c>
+      <c r="C17" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" t="s">
+        <v>5</v>
+      </c>
+      <c r="E17" s="1">
+        <v>400</v>
+      </c>
+      <c r="F17" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>3.1108832157324899</v>
+      </c>
+      <c r="B18">
+        <v>0.74043038155819096</v>
+      </c>
+      <c r="C18" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" t="s">
+        <v>5</v>
+      </c>
+      <c r="E18" s="1">
+        <v>400</v>
+      </c>
+      <c r="F18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>6.7629119578067902</v>
+      </c>
+      <c r="B19">
+        <v>0.75192312278753104</v>
+      </c>
+      <c r="C19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" t="s">
+        <v>5</v>
+      </c>
+      <c r="E19" s="1">
+        <v>400</v>
+      </c>
+      <c r="F19" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>12.081926495790499</v>
+      </c>
+      <c r="B20">
+        <v>0.57039627674978799</v>
+      </c>
+      <c r="C20" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" t="s">
+        <v>5</v>
+      </c>
+      <c r="E20" s="1">
+        <v>400</v>
+      </c>
+      <c r="F20" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>16.448377721825999</v>
+      </c>
+      <c r="B21">
+        <v>7.0594909150378304E-2</v>
+      </c>
+      <c r="C21" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" t="s">
+        <v>5</v>
+      </c>
+      <c r="E21" s="1">
+        <v>400</v>
+      </c>
+      <c r="F21" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>21.331831949493498</v>
+      </c>
+      <c r="B22">
+        <v>-0.47793510887304103</v>
+      </c>
+      <c r="C22" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22" t="s">
+        <v>5</v>
+      </c>
+      <c r="E22" s="1">
+        <v>400</v>
+      </c>
+      <c r="F22" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>26.7731740639916</v>
+      </c>
+      <c r="B23">
+        <v>-1.0670270215020401</v>
+      </c>
+      <c r="C23" t="s">
+        <v>6</v>
+      </c>
+      <c r="D23" t="s">
+        <v>5</v>
+      </c>
+      <c r="E23" s="1">
+        <v>400</v>
+      </c>
+      <c r="F23" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>-4.5612745181545904</v>
+      </c>
+      <c r="B24">
+        <v>0.21391687421424299</v>
+      </c>
+      <c r="C24" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24" t="s">
+        <v>5</v>
+      </c>
+      <c r="E24" s="1">
+        <v>730</v>
+      </c>
+      <c r="F24" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>-0.72381919340936196</v>
+      </c>
+      <c r="B25">
+        <v>0.920448575332104</v>
+      </c>
+      <c r="C25" t="s">
+        <v>6</v>
+      </c>
+      <c r="D25" t="s">
+        <v>5</v>
+      </c>
+      <c r="E25" s="1">
+        <v>730</v>
+      </c>
+      <c r="F25" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>4.9948314690961304</v>
+      </c>
+      <c r="B26">
+        <v>1.1507490451675699</v>
+      </c>
+      <c r="C26" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" t="s">
+        <v>5</v>
+      </c>
+      <c r="E26" s="1">
+        <v>730</v>
+      </c>
+      <c r="F26" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>9.0864817534164395</v>
+      </c>
+      <c r="B27">
+        <v>1.1440561894605501</v>
+      </c>
+      <c r="C27" t="s">
+        <v>6</v>
+      </c>
+      <c r="D27" t="s">
+        <v>5</v>
+      </c>
+      <c r="E27" s="1">
+        <v>730</v>
+      </c>
+      <c r="F27" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>14.118157318224</v>
+      </c>
+      <c r="B28">
+        <v>0.893133383530887</v>
+      </c>
+      <c r="C28" t="s">
+        <v>6</v>
+      </c>
+      <c r="D28" t="s">
+        <v>5</v>
+      </c>
+      <c r="E28" s="1">
+        <v>730</v>
+      </c>
+      <c r="F28" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>18.185767290047501</v>
+      </c>
+      <c r="B29">
+        <v>0.62963847540263096</v>
+      </c>
+      <c r="C29" t="s">
+        <v>6</v>
+      </c>
+      <c r="D29" t="s">
+        <v>5</v>
+      </c>
+      <c r="E29" s="1">
+        <v>730</v>
+      </c>
+      <c r="F29" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>23.992020633238699</v>
+      </c>
+      <c r="B30">
+        <v>8.14375807050602E-2</v>
+      </c>
+      <c r="C30" t="s">
+        <v>6</v>
+      </c>
+      <c r="D30" t="s">
+        <v>5</v>
+      </c>
+      <c r="E30" s="1">
+        <v>730</v>
+      </c>
+      <c r="F30" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>28.791470050118001</v>
+      </c>
+      <c r="B31">
+        <v>-0.93587239827329405</v>
+      </c>
+      <c r="C31" t="s">
+        <v>6</v>
+      </c>
+      <c r="D31" t="s">
+        <v>5</v>
+      </c>
+      <c r="E31" s="1">
+        <v>730</v>
+      </c>
+      <c r="F31" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>-3.2525765995359599</v>
+      </c>
+      <c r="B32">
+        <v>0.47932928345831599</v>
+      </c>
+      <c r="C32" t="s">
+        <v>6</v>
+      </c>
+      <c r="D32" t="s">
+        <v>5</v>
+      </c>
+      <c r="E32" s="1">
+        <v>970</v>
+      </c>
+      <c r="F32" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>1.74688167573515</v>
+      </c>
+      <c r="B33">
+        <v>1.1699710739437199</v>
+      </c>
+      <c r="C33" t="s">
+        <v>6</v>
+      </c>
+      <c r="D33" t="s">
+        <v>5</v>
+      </c>
+      <c r="E33" s="1">
+        <v>970</v>
+      </c>
+      <c r="F33" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>6.6913906652992896</v>
+      </c>
+      <c r="B34">
+        <v>1.2736367446091501</v>
+      </c>
+      <c r="C34" t="s">
+        <v>6</v>
+      </c>
+      <c r="D34" t="s">
+        <v>5</v>
+      </c>
+      <c r="E34" s="1">
+        <v>970</v>
+      </c>
+      <c r="F34" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>11.028350260811401</v>
+      </c>
+      <c r="B35">
+        <v>1.31594442381272</v>
+      </c>
+      <c r="C35" t="s">
+        <v>6</v>
+      </c>
+      <c r="D35" t="s">
+        <v>5</v>
+      </c>
+      <c r="E35" s="1">
+        <v>970</v>
+      </c>
+      <c r="F35" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>15.5705519800209</v>
+      </c>
+      <c r="B36">
+        <v>0.97924921722480196</v>
+      </c>
+      <c r="C36" t="s">
+        <v>6</v>
+      </c>
+      <c r="D36" t="s">
+        <v>5</v>
+      </c>
+      <c r="E36" s="1">
+        <v>970</v>
+      </c>
+      <c r="F36" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>19.578524532634599</v>
+      </c>
+      <c r="B37">
+        <v>0.93584173460939601</v>
+      </c>
+      <c r="C37" t="s">
+        <v>6</v>
+      </c>
+      <c r="D37" t="s">
+        <v>5</v>
+      </c>
+      <c r="E37" s="1">
+        <v>970</v>
+      </c>
+      <c r="F37" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>25.705751481225299</v>
+      </c>
+      <c r="B38">
+        <v>0.38775531759038101</v>
+      </c>
+      <c r="C38" t="s">
+        <v>6</v>
+      </c>
+      <c r="D38" t="s">
+        <v>5</v>
+      </c>
+      <c r="E38" s="1">
+        <v>970</v>
+      </c>
+      <c r="F38" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>